<commit_message>
made lots of updates to scripts and files
</commit_message>
<xml_diff>
--- a/dcor-wpac/dcor.wpac.qa-qc.xlsx
+++ b/dcor-wpac/dcor.wpac.qa-qc.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aonoufriou/Documents/GitHub/Turtle_GTseq_SNPs/dcor-wpac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE5BDFA-4872-0A4A-A12E-9DB57B0FFA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EABD59-EC8C-3548-9C5F-33C6AA381074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="920" windowWidth="17060" windowHeight="21260" activeTab="1" xr2:uid="{82AAAB80-8365-2249-8220-88EE1B49404F}"/>
+    <workbookView xWindow="6700" yWindow="3560" windowWidth="14400" windowHeight="9660" activeTab="1" xr2:uid="{82AAAB80-8365-2249-8220-88EE1B49404F}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleData" sheetId="1" r:id="rId1"/>
     <sheet name="ChangeIssueNotes" sheetId="2" r:id="rId2"/>
-    <sheet name="labels-wreps" sheetId="3" r:id="rId3"/>
-    <sheet name="labels-merged" sheetId="4" r:id="rId4"/>
-    <sheet name="Summary Files" sheetId="5" r:id="rId5"/>
-    <sheet name="wreps-pass1-mismatches" sheetId="6" r:id="rId6"/>
-    <sheet name="merged-pass1-genos.to.check" sheetId="7" r:id="rId7"/>
+    <sheet name="labels-merged-nodups" sheetId="10" r:id="rId3"/>
+    <sheet name="labels-wreps" sheetId="3" r:id="rId4"/>
+    <sheet name="labels-merged" sheetId="4" r:id="rId5"/>
+    <sheet name="Summary Files" sheetId="5" r:id="rId6"/>
+    <sheet name="genos_to_change" sheetId="9" r:id="rId7"/>
+    <sheet name="merged-pass1-genos.to.check" sheetId="7" r:id="rId8"/>
+    <sheet name="wreps-pass1-mismatches" sheetId="6" r:id="rId9"/>
+    <sheet name="wreps-pass1-genos.to.check" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'wreps-pass1-mismatches'!$A$1:$L$453</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'wreps-pass1-mismatches'!$A$1:$L$453</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9232" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9863" uniqueCount="1348">
   <si>
     <t>sort</t>
   </si>
@@ -3922,9 +3925,6 @@
     <t>Justification</t>
   </si>
   <si>
-    <t>When Ns removed, &gt;20 reads, only C's, homozygote</t>
-  </si>
-  <si>
     <t xml:space="preserve">When Ns removed, &lt;20 reads remaining. No genotype. </t>
   </si>
   <si>
@@ -3983,13 +3983,121 @@
   </si>
   <si>
     <t>Becomes NA because MAF (N) is 20.2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 8/8/25 I emailed Karen about locus 016 explaining the situation with it. </t>
+  </si>
+  <si>
+    <t>For sample 12527 at locus016, a "C/N" genotype for the sample and "C/C" for its replicate. When merged, the genotype became an NA due to a high minor allele frequency (20.2%) of "N," which is not a real haplotype.</t>
+  </si>
+  <si>
+    <t>I wondered if im losing data unncessarily by calling it an NA and whether I should call it a C/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karen agrees that it looks like the sample is a C/C but worries that the N values could bias the genotypes at the locus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Issue would be if there was a sample that was not replicated and had a read count similar to the merged data for 12527 (NA genotype). It would be filtered out without ever having a chance to scrutinize it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Best to add a step before merging replicates to look at questionable haplotypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -some loci wong get filtered at the 90% step but get flagged as problematic in the questionable haplotypes. Removing loci early in the process can make the rest of it easier. </t>
+  </si>
+  <si>
+    <t>G/N</t>
+  </si>
+  <si>
+    <t>Dropping locus016</t>
+  </si>
+  <si>
+    <t>Remove locus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed genotype for individual z0062687 at locus 069 to NA. When Ns removed, &lt;20 reads remaining. No genotype. </t>
+  </si>
+  <si>
+    <t>Worked through up to the LD, HWE and heterozygosity script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think some work needs to be done on the gtypes file because I'm not able to filter out by population. </t>
+  </si>
+  <si>
+    <t>Fixed and updated the make gtypes script and reran</t>
+  </si>
+  <si>
+    <t>ids.1</t>
+  </si>
+  <si>
+    <t>ids.2</t>
+  </si>
+  <si>
+    <t>strata.1</t>
+  </si>
+  <si>
+    <t>strata.2</t>
+  </si>
+  <si>
+    <t>mismatch.loci</t>
+  </si>
+  <si>
+    <t>num.loci.genotyped</t>
+  </si>
+  <si>
+    <t>num.loci.shared</t>
+  </si>
+  <si>
+    <t>prop.loci.shared</t>
+  </si>
+  <si>
+    <t>&lt;NA&gt;</t>
+  </si>
+  <si>
+    <t>Ran the check duplicates script:</t>
+  </si>
+  <si>
+    <t>Previous conversations with Amy Frey decided this:</t>
+  </si>
+  <si>
+    <t>Merge: 26457 and 40945 and call the sample 26457</t>
+  </si>
+  <si>
+    <t>Merge: 26450 and 40943 and call the sample 26450</t>
+  </si>
+  <si>
+    <t>Keep: 12504</t>
+  </si>
+  <si>
+    <t>Delete: 12514</t>
+  </si>
+  <si>
+    <t>Matched with microsats (one marker different, but marker is difficult). Different field IDs, collected one day apart</t>
+  </si>
+  <si>
+    <t>Matched with microsats, same field ID and same turtle ID</t>
+  </si>
+  <si>
+    <t>samtools merge 26457_merged2.sam 26457_merged.sam 40945_mapped2ref.sam</t>
+  </si>
+  <si>
+    <t>samtools merge 26450_merged2.sam 26450_merged.sam 40943_mapped2ref.sam</t>
+  </si>
+  <si>
+    <t>Need to go back through the genotyping script with updated sample list: "dcor.wpac.labels_zpad_merged_nodups.txt"</t>
+  </si>
+  <si>
+    <t>Done all through creating gtypes</t>
+  </si>
+  <si>
+    <t>No duplicate pairs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4017,8 +4125,15 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4031,8 +4146,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4040,18 +4161,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27126,12 +27283,311 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6393F95A-46DC-B742-81B4-7A390994A7CA}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C2" t="s">
+        <v>563</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>103</v>
+      </c>
+      <c r="J2">
+        <v>65</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C3" t="s">
+        <v>879</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>83</v>
+      </c>
+      <c r="J3">
+        <v>64</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>68</v>
+      </c>
+      <c r="J4">
+        <v>56</v>
+      </c>
+      <c r="K4">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>55</v>
+      </c>
+      <c r="J5">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C6" t="s">
+        <v>549</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C7" t="s">
+        <v>685</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0F25FC-ACC9-FC49-90CA-EADA62E1BF7E}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:N31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27144,7 +27600,7 @@
         <v>46606</v>
       </c>
       <c r="B1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -27185,10 +27641,10 @@
         <v>1142</v>
       </c>
       <c r="N2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="O2" t="s">
         <v>1297</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1298</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -27267,23 +27723,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I5" s="4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I5">
         <f>SUM(I3:I4)</f>
         <v>231</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <f>SUM(J3:J4)</f>
         <v>96</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5">
         <f>J5/SUM(I5:J5)</f>
         <v>0.29357798165137616</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -27363,23 +27819,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I8" s="4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I8">
         <f>SUM(I6:I7)</f>
         <v>335</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <f>SUM(J6:J7)</f>
         <v>130</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <f>J8/SUM(I8:J8)</f>
         <v>0.27956989247311825</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" t="s">
         <v>60</v>
       </c>
     </row>
@@ -27459,23 +27915,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I11" s="4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I11">
         <f>SUM(I9:I10)</f>
         <v>442</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <f>SUM(J9:J10)</f>
         <v>127</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <f>J11/SUM(I11:J11)</f>
         <v>0.22319859402460457</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -27555,9 +28011,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
-        <v>1296</v>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>1295</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -27636,24 +28092,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I17" s="4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I17">
         <f>SUM(I15:I16)</f>
         <v>44</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17">
         <f>SUM(J15:J16)</f>
         <v>21</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17">
         <f>J17/SUM(I17:J17)</f>
         <v>0.32307692307692309</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>1299</v>
+      <c r="O17" t="s">
+        <v>1298</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -27732,24 +28188,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I20" s="4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I20">
         <f>SUM(I18:I19)</f>
         <v>83</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20">
         <f>SUM(J18:J19)</f>
         <v>56</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20">
         <f>J20/SUM(I20:J20)</f>
         <v>0.40287769784172661</v>
       </c>
-      <c r="O20" s="4" t="s">
-        <v>1299</v>
+      <c r="O20" t="s">
+        <v>1298</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -27828,35 +28284,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="I23" s="4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I23">
         <f>SUM(I21:I22)</f>
         <v>93</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23">
         <f>SUM(J21:J22)</f>
         <v>34</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23">
         <f>J23/SUM(I23:J23)</f>
         <v>0.26771653543307089</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="O23" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -27864,34 +28319,34 @@
         <v>1131</v>
       </c>
       <c r="C28" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D28" t="s">
         <v>1133</v>
       </c>
       <c r="E28" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F28" t="s">
         <v>1302</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>1303</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>1304</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>1305</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>1306</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>1307</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>1308</v>
-      </c>
-      <c r="L28" t="s">
-        <v>1309</v>
       </c>
       <c r="M28" t="s">
         <v>1142</v>
@@ -27899,140 +28354,401 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1310</v>
-      </c>
-      <c r="B29" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>879</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>1289</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="4" t="s">
         <v>1180</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="H29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" s="4">
         <v>83</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="4">
         <v>64</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="4">
         <v>1</v>
       </c>
-      <c r="L29" s="5">
-        <v>0</v>
-      </c>
-      <c r="M29" s="5">
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>882</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>1181</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>1180</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="H30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="4">
         <v>181</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4">
         <v>3</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="4">
         <v>2</v>
       </c>
-      <c r="L30" s="5">
-        <v>0</v>
-      </c>
-      <c r="M30" s="5">
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="4">
+        <v>264</v>
+      </c>
+      <c r="J31" s="4">
+        <v>67</v>
+      </c>
+      <c r="K31" s="4">
+        <v>3</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
         <v>1311</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>879</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>1158</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>1180</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="5">
-        <v>264</v>
-      </c>
-      <c r="J31" s="5">
-        <v>67</v>
-      </c>
-      <c r="K31" s="5">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>45882</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>45883</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1330</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1331</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1332</v>
+      </c>
+      <c r="J49" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D50" t="s">
+        <v>950</v>
+      </c>
+      <c r="E50" t="s">
+        <v>939</v>
+      </c>
+      <c r="F50" t="s">
+        <v>939</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H50">
+        <v>159</v>
+      </c>
+      <c r="I50">
+        <v>159</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L50" s="9" t="s">
+        <v>950</v>
+      </c>
+      <c r="M50" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>775</v>
+      </c>
+      <c r="D51" t="s">
+        <v>712</v>
+      </c>
+      <c r="E51" t="s">
+        <v>668</v>
+      </c>
+      <c r="F51" t="s">
+        <v>668</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H51">
+        <v>154</v>
+      </c>
+      <c r="I51">
+        <v>154</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="M51" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52">
         <v>3</v>
       </c>
-      <c r="L31" s="5">
-        <v>0</v>
-      </c>
-      <c r="M31" s="5">
-        <v>0</v>
-      </c>
-      <c r="N31" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="C52" t="s">
+        <v>983</v>
+      </c>
+      <c r="D52" t="s">
+        <v>944</v>
+      </c>
+      <c r="E52" t="s">
+        <v>939</v>
+      </c>
+      <c r="F52" t="s">
+        <v>939</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H52">
+        <v>138</v>
+      </c>
+      <c r="I52">
+        <v>138</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>983</v>
+      </c>
+      <c r="L52" s="9" t="s">
+        <v>944</v>
+      </c>
+      <c r="M52" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>1347</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28040,11 +28756,1925 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD027E0-DFA5-E34D-9D2F-C27719CC1FA6}">
+  <dimension ref="A1:C172"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B2" t="s">
+        <v>835</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B3" t="s">
+        <v>839</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B4" t="s">
+        <v>806</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B5" t="s">
+        <v>843</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>847</v>
+      </c>
+      <c r="B6" t="s">
+        <v>848</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>816</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B8" t="s">
+        <v>824</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B10" t="s">
+        <v>674</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B11" t="s">
+        <v>682</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>735</v>
+      </c>
+      <c r="B12" t="s">
+        <v>736</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>738</v>
+      </c>
+      <c r="B13" t="s">
+        <v>739</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>741</v>
+      </c>
+      <c r="B14" t="s">
+        <v>742</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>744</v>
+      </c>
+      <c r="B15" t="s">
+        <v>745</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>747</v>
+      </c>
+      <c r="B16" t="s">
+        <v>748</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>750</v>
+      </c>
+      <c r="B17" t="s">
+        <v>751</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B18" t="s">
+        <v>688</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>884</v>
+      </c>
+      <c r="B19" t="s">
+        <v>885</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>753</v>
+      </c>
+      <c r="B20" t="s">
+        <v>754</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B21" t="s">
+        <v>694</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>756</v>
+      </c>
+      <c r="B22" t="s">
+        <v>757</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>759</v>
+      </c>
+      <c r="B23" t="s">
+        <v>760</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>762</v>
+      </c>
+      <c r="B24" t="s">
+        <v>763</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>699</v>
+      </c>
+      <c r="B25" t="s">
+        <v>700</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>765</v>
+      </c>
+      <c r="B26" t="s">
+        <v>766</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>768</v>
+      </c>
+      <c r="B27" t="s">
+        <v>769</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B28" t="s">
+        <v>706</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>887</v>
+      </c>
+      <c r="B29" t="s">
+        <v>888</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>771</v>
+      </c>
+      <c r="B30" t="s">
+        <v>772</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>774</v>
+      </c>
+      <c r="B31" t="s">
+        <v>775</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>890</v>
+      </c>
+      <c r="B32" t="s">
+        <v>891</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B33" t="s">
+        <v>869</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>777</v>
+      </c>
+      <c r="B34" t="s">
+        <v>778</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>780</v>
+      </c>
+      <c r="B35" t="s">
+        <v>781</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>783</v>
+      </c>
+      <c r="B36" t="s">
+        <v>784</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B37" t="s">
+        <v>718</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B38" t="s">
+        <v>724</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B39" t="s">
+        <v>730</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>786</v>
+      </c>
+      <c r="B40" t="s">
+        <v>787</v>
+      </c>
+      <c r="C40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>789</v>
+      </c>
+      <c r="B41" t="s">
+        <v>790</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>792</v>
+      </c>
+      <c r="B42" t="s">
+        <v>793</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>795</v>
+      </c>
+      <c r="B43" t="s">
+        <v>796</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>798</v>
+      </c>
+      <c r="B44" t="s">
+        <v>799</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B45" t="s">
+        <v>879</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>802</v>
+      </c>
+      <c r="B46" t="s">
+        <v>803</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>910</v>
+      </c>
+      <c r="B47" t="s">
+        <v>911</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>914</v>
+      </c>
+      <c r="B48" t="s">
+        <v>915</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B49" t="s">
+        <v>899</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>918</v>
+      </c>
+      <c r="B50" t="s">
+        <v>919</v>
+      </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>922</v>
+      </c>
+      <c r="B51" t="s">
+        <v>923</v>
+      </c>
+      <c r="C51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>926</v>
+      </c>
+      <c r="B52" t="s">
+        <v>927</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>930</v>
+      </c>
+      <c r="B53" t="s">
+        <v>931</v>
+      </c>
+      <c r="C53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B54" t="s">
+        <v>983</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B55" t="s">
+        <v>992</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B56" t="s">
+        <v>999</v>
+      </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B60" t="s">
+        <v>954</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>961</v>
+      </c>
+      <c r="B61" t="s">
+        <v>962</v>
+      </c>
+      <c r="C61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>965</v>
+      </c>
+      <c r="B62" t="s">
+        <v>966</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>969</v>
+      </c>
+      <c r="B63" t="s">
+        <v>970</v>
+      </c>
+      <c r="C63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>974</v>
+      </c>
+      <c r="B64" t="s">
+        <v>975</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>978</v>
+      </c>
+      <c r="B65" t="s">
+        <v>979</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B66" t="s">
+        <v>612</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" t="s">
+        <v>317</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>320</v>
+      </c>
+      <c r="B68" t="s">
+        <v>321</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>324</v>
+      </c>
+      <c r="B69" t="s">
+        <v>325</v>
+      </c>
+      <c r="C69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B70" t="s">
+        <v>238</v>
+      </c>
+      <c r="C70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>328</v>
+      </c>
+      <c r="B71" t="s">
+        <v>329</v>
+      </c>
+      <c r="C71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B72" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" t="s">
+        <v>187</v>
+      </c>
+      <c r="C73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" t="s">
+        <v>191</v>
+      </c>
+      <c r="C74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>934</v>
+      </c>
+      <c r="B80" t="s">
+        <v>935</v>
+      </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>664</v>
+      </c>
+      <c r="B81" t="s">
+        <v>665</v>
+      </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>893</v>
+      </c>
+      <c r="B82" t="s">
+        <v>894</v>
+      </c>
+      <c r="C82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B83" t="s">
+        <v>852</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>859</v>
+      </c>
+      <c r="B84" t="s">
+        <v>860</v>
+      </c>
+      <c r="C84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B86" t="s">
+        <v>256</v>
+      </c>
+      <c r="C86" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B87" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B88" t="s">
+        <v>271</v>
+      </c>
+      <c r="C88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B89" t="s">
+        <v>278</v>
+      </c>
+      <c r="C89" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B90" t="s">
+        <v>285</v>
+      </c>
+      <c r="C90" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>332</v>
+      </c>
+      <c r="B91" t="s">
+        <v>333</v>
+      </c>
+      <c r="C91" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B92" t="s">
+        <v>398</v>
+      </c>
+      <c r="C92" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>450</v>
+      </c>
+      <c r="B93" t="s">
+        <v>451</v>
+      </c>
+      <c r="C93" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B94" t="s">
+        <v>409</v>
+      </c>
+      <c r="C94" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B95" t="s">
+        <v>416</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B96" t="s">
+        <v>423</v>
+      </c>
+      <c r="C96" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B97" t="s">
+        <v>430</v>
+      </c>
+      <c r="C97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B98" t="s">
+        <v>437</v>
+      </c>
+      <c r="C98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B99" t="s">
+        <v>444</v>
+      </c>
+      <c r="C99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B100" t="s">
+        <v>292</v>
+      </c>
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>336</v>
+      </c>
+      <c r="B101" t="s">
+        <v>337</v>
+      </c>
+      <c r="C101" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B102" t="s">
+        <v>301</v>
+      </c>
+      <c r="C102" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B103" t="s">
+        <v>309</v>
+      </c>
+      <c r="C103" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>341</v>
+      </c>
+      <c r="B104" t="s">
+        <v>342</v>
+      </c>
+      <c r="C104" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>346</v>
+      </c>
+      <c r="B105" t="s">
+        <v>347</v>
+      </c>
+      <c r="C105" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>351</v>
+      </c>
+      <c r="B106" t="s">
+        <v>352</v>
+      </c>
+      <c r="C106" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>356</v>
+      </c>
+      <c r="B107" t="s">
+        <v>357</v>
+      </c>
+      <c r="C107" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>361</v>
+      </c>
+      <c r="B108" t="s">
+        <v>362</v>
+      </c>
+      <c r="C108" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>366</v>
+      </c>
+      <c r="B109" t="s">
+        <v>367</v>
+      </c>
+      <c r="C109" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>371</v>
+      </c>
+      <c r="B110" t="s">
+        <v>372</v>
+      </c>
+      <c r="C110" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>376</v>
+      </c>
+      <c r="B111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C111" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>381</v>
+      </c>
+      <c r="B112" t="s">
+        <v>382</v>
+      </c>
+      <c r="C112" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B114" t="s">
+        <v>213</v>
+      </c>
+      <c r="C114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B115" t="s">
+        <v>163</v>
+      </c>
+      <c r="C115" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B116" t="s">
+        <v>171</v>
+      </c>
+      <c r="C116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>222</v>
+      </c>
+      <c r="B117" t="s">
+        <v>223</v>
+      </c>
+      <c r="C117" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B118" t="s">
+        <v>636</v>
+      </c>
+      <c r="C118" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>656</v>
+      </c>
+      <c r="B119" t="s">
+        <v>657</v>
+      </c>
+      <c r="C119" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>660</v>
+      </c>
+      <c r="B120" t="s">
+        <v>661</v>
+      </c>
+      <c r="C120" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B121" t="s">
+        <v>650</v>
+      </c>
+      <c r="C121" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" t="s">
+        <v>104</v>
+      </c>
+      <c r="C122" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>113</v>
+      </c>
+      <c r="B123" t="s">
+        <v>114</v>
+      </c>
+      <c r="C123" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>98</v>
+      </c>
+      <c r="B124" t="s">
+        <v>99</v>
+      </c>
+      <c r="C124" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>108</v>
+      </c>
+      <c r="B125" t="s">
+        <v>109</v>
+      </c>
+      <c r="C125" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>202</v>
+      </c>
+      <c r="B126" t="s">
+        <v>203</v>
+      </c>
+      <c r="C126" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B127" t="s">
+        <v>195</v>
+      </c>
+      <c r="C127" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B128" t="s">
+        <v>387</v>
+      </c>
+      <c r="C128" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>207</v>
+      </c>
+      <c r="B129" t="s">
+        <v>208</v>
+      </c>
+      <c r="C129" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>157</v>
+      </c>
+      <c r="B130" t="s">
+        <v>158</v>
+      </c>
+      <c r="C130" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" t="s">
+        <v>135</v>
+      </c>
+      <c r="C131" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B132" t="s">
+        <v>87</v>
+      </c>
+      <c r="C132" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>176</v>
+      </c>
+      <c r="B133" t="s">
+        <v>177</v>
+      </c>
+      <c r="C133" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B134" t="s">
+        <v>127</v>
+      </c>
+      <c r="C134" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>152</v>
+      </c>
+      <c r="B135" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>139</v>
+      </c>
+      <c r="B136" t="s">
+        <v>140</v>
+      </c>
+      <c r="C136" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B137" t="s">
+        <v>119</v>
+      </c>
+      <c r="C137" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B138" t="s">
+        <v>145</v>
+      </c>
+      <c r="C138" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B139" t="s">
+        <v>580</v>
+      </c>
+      <c r="C139" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B140" t="s">
+        <v>602</v>
+      </c>
+      <c r="C140" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B141" t="s">
+        <v>608</v>
+      </c>
+      <c r="C141" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B142" t="s">
+        <v>592</v>
+      </c>
+      <c r="C142" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B143" t="s">
+        <v>630</v>
+      </c>
+      <c r="C143" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B144" t="s">
+        <v>622</v>
+      </c>
+      <c r="C144" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B145" t="s">
+        <v>503</v>
+      </c>
+      <c r="C145" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B146" t="s">
+        <v>508</v>
+      </c>
+      <c r="C146" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B147" t="s">
+        <v>512</v>
+      </c>
+      <c r="C147" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B148" t="s">
+        <v>516</v>
+      </c>
+      <c r="C148" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B149" t="s">
+        <v>520</v>
+      </c>
+      <c r="C149" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B150" t="s">
+        <v>524</v>
+      </c>
+      <c r="C150" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B151" t="s">
+        <v>529</v>
+      </c>
+      <c r="C151" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B152" t="s">
+        <v>533</v>
+      </c>
+      <c r="C152" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B153" t="s">
+        <v>537</v>
+      </c>
+      <c r="C153" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B154" t="s">
+        <v>541</v>
+      </c>
+      <c r="C154" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B155" t="s">
+        <v>545</v>
+      </c>
+      <c r="C155" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B156" t="s">
+        <v>549</v>
+      </c>
+      <c r="C156" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B157" t="s">
+        <v>553</v>
+      </c>
+      <c r="C157" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B158" t="s">
+        <v>559</v>
+      </c>
+      <c r="C158" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B159" t="s">
+        <v>563</v>
+      </c>
+      <c r="C159" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B160" t="s">
+        <v>567</v>
+      </c>
+      <c r="C160" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B161" t="s">
+        <v>572</v>
+      </c>
+      <c r="C161" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B162" t="s">
+        <v>576</v>
+      </c>
+      <c r="C162" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B163" t="s">
+        <v>455</v>
+      </c>
+      <c r="C163" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B164" t="s">
+        <v>469</v>
+      </c>
+      <c r="C164" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B165" t="s">
+        <v>473</v>
+      </c>
+      <c r="C165" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B166" t="s">
+        <v>477</v>
+      </c>
+      <c r="C166" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B167" t="s">
+        <v>481</v>
+      </c>
+      <c r="C167" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B168" t="s">
+        <v>485</v>
+      </c>
+      <c r="C168" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B169" t="s">
+        <v>489</v>
+      </c>
+      <c r="C169" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B170" t="s">
+        <v>493</v>
+      </c>
+      <c r="C170" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B171" t="s">
+        <v>499</v>
+      </c>
+      <c r="C171" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B172" t="s">
+        <v>864</v>
+      </c>
+      <c r="C172" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C173">
+    <sortCondition ref="B1:B173"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B863A1-28B0-034A-A164-979ADC1A5787}">
   <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="I266" sqref="I266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30554,12 +33184,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412E7743-53EA-E94C-A063-C2D445A2B0E2}">
   <dimension ref="A1:C175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32494,7 +35124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D26B8FF-B51C-0A4C-9DAD-D9887254401E}">
   <dimension ref="A1:A27"/>
   <sheetViews>
@@ -32632,7 +35262,294 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDCA9FF-FC48-2B43-BD0F-BF19C6923D2E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17F8E18-BCD7-0841-9E56-E37D35FE2EA7}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="43.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C2" t="s">
+        <v>563</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>103</v>
+      </c>
+      <c r="J2">
+        <v>65</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C3" t="s">
+        <v>485</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>55</v>
+      </c>
+      <c r="J3">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>549</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>398</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B4303A-592C-BE42-BA9A-8A436E462A9E}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L453"/>
@@ -49883,254 +52800,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17F8E18-BCD7-0841-9E56-E37D35FE2EA7}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="15" max="15" width="43.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1135</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1136</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1137</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1138</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1139</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1141</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1142</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1290</v>
-      </c>
-      <c r="O1" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C2" t="s">
-        <v>563</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1158</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2">
-        <v>103</v>
-      </c>
-      <c r="J2">
-        <v>65</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1181</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C3" t="s">
-        <v>485</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1158</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3">
-        <v>55</v>
-      </c>
-      <c r="J3">
-        <v>38</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1181</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C4" t="s">
-        <v>549</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1158</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4">
-        <v>23</v>
-      </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1181</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1240</v>
-      </c>
-      <c r="C5" t="s">
-        <v>398</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1155</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1156</v>
-      </c>
-      <c r="G5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5">
-        <v>14</v>
-      </c>
-      <c r="J5">
-        <v>11</v>
-      </c>
-      <c r="K5">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5" t="s">
-        <v>60</v>
-      </c>
-      <c r="O5" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>